<commit_message>
fix: reorg files and add interactive blocks to Step2b
</commit_message>
<xml_diff>
--- a/data/sample_sheet_test.xlsx
+++ b/data/sample_sheet_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdivoll/obitools2-pipeline/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B57A3D9-2E92-9240-ABD0-55FA947F51D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8184C6-F624-4941-A62C-AE55EC87C647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="1600" windowWidth="16460" windowHeight="16940" xr2:uid="{72C51BDD-6642-E64B-94FB-AADA16EE7827}"/>
   </bookViews>
@@ -66,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{FE31806E-AF55-DA48-A343-8A0A689E5CD2}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{FE31806E-AF55-DA48-A343-8A0A689E5CD2}">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{37AECCA5-E90C-334C-A620-D2A20DAA0DD3}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{37AECCA5-E90C-334C-A620-D2A20DAA0DD3}">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{DCAE1CC7-4B70-414B-B5CA-984DE5F29D60}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{DCAE1CC7-4B70-414B-B5CA-984DE5F29D60}">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{6C833794-5C3F-2049-AA46-677DD7EC42D2}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{6C833794-5C3F-2049-AA46-677DD7EC42D2}">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{40E4DBE3-45E3-BB45-8AAA-8B73BA649333}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{40E4DBE3-45E3-BB45-8AAA-8B73BA649333}">
       <text>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{3C287F53-2999-6C4F-8403-16E2AB2B6932}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{3C287F53-2999-6C4F-8403-16E2AB2B6932}">
       <text>
         <r>
           <rPr>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>Plate#</t>
   </si>
@@ -184,9 +184,6 @@
     <t>PCR date</t>
   </si>
   <si>
-    <t>seq date</t>
-  </si>
-  <si>
     <t>BLA20211203.A</t>
   </si>
   <si>
@@ -257,6 +254,18 @@
   </si>
   <si>
     <t>extraction group 3</t>
+  </si>
+  <si>
+    <t>Seq date</t>
+  </si>
+  <si>
+    <t>Contol</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -643,21 +652,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F3964E-8FD1-2A47-B519-6732111C8D86}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="3" max="4" width="16" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -667,259 +676,280 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
+      <c r="M1" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="6">
+      <c r="J2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="6">
         <v>44767</v>
       </c>
-      <c r="K2" s="6">
+      <c r="L2" s="6">
         <v>44778</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>44847</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="6">
+      <c r="J3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="6">
         <v>44767</v>
       </c>
-      <c r="K3" s="6">
+      <c r="L3" s="6">
         <v>44778</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="5">
         <v>44847</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="6">
+      <c r="J4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="6">
         <v>44767</v>
       </c>
-      <c r="K4" s="6">
+      <c r="L4" s="6">
         <v>44778</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>44847</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="K5" s="5">
         <v>44774</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>44783</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>44847</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>44774</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>44783</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>44847</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="K7" s="5">
         <v>44774</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L7" s="5">
         <v>44783</v>
       </c>
-      <c r="L7" s="5">
+      <c r="M7" s="5">
         <v>44847</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: update here paths and copying
</commit_message>
<xml_diff>
--- a/data/sample_sheet_test.xlsx
+++ b/data/sample_sheet_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdivoll/obitools2-pipeline/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8184C6-F624-4941-A62C-AE55EC87C647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1116DD1-F612-5442-B42D-061BC970AAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2600" yWindow="1600" windowWidth="16460" windowHeight="16940" xr2:uid="{72C51BDD-6642-E64B-94FB-AADA16EE7827}"/>
   </bookViews>
@@ -259,13 +259,13 @@
     <t>Seq date</t>
   </si>
   <si>
-    <t>Contol</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Control</t>
   </si>
 </sst>
 </file>
@@ -655,7 +655,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +677,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -718,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>23</v>
@@ -759,7 +759,7 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
@@ -800,7 +800,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>25</v>
@@ -841,7 +841,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>26</v>
@@ -882,7 +882,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>27</v>
@@ -923,7 +923,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>

</xml_diff>